<commit_message>
adaptAandEPS_OUT (ignore opp) is the best yet: only need to improve DIFF_PROP_OUT for C and E
</commit_message>
<xml_diff>
--- a/ampl/output/aushistoric/agg-gladlab-SHRnoEPSknitro-0-aus-EPS_OUT_C_E_700-historic.xlsx
+++ b/ampl/output/aushistoric/agg-gladlab-SHRnoEPSknitro-0-aus-EPS_OUT_C_E_700-historic.xlsx
@@ -184,16 +184,16 @@
         <v>19</v>
       </c>
       <c r="D2" t="n">
-        <v>11.800781901324195</v>
+        <v>11.64488325573536</v>
       </c>
       <c r="E2" t="n">
-        <v>5.4938586477977642</v>
+        <v>5.3834807507191291</v>
       </c>
       <c r="F2" t="n">
-        <v>1.2854159340326903</v>
+        <v>1.2606494691624988</v>
       </c>
       <c r="G2" t="n">
-        <v>2.9012258906706214</v>
+        <v>2.8889835156439041</v>
       </c>
     </row>
     <row r="3">
@@ -204,19 +204,19 @@
         <v>1</v>
       </c>
       <c r="C3" t="n">
-        <v>18.051841462193643</v>
+        <v>18.051841500652817</v>
       </c>
       <c r="D3" t="n">
-        <v>11.851947805120064</v>
+        <v>11.694962128429422</v>
       </c>
       <c r="E3" t="n">
-        <v>5.5279594920202948</v>
+        <v>5.4167716717953338</v>
       </c>
       <c r="F3" t="n">
-        <v>1.2903457798170526</v>
+        <v>1.2653896663194277</v>
       </c>
       <c r="G3" t="n">
-        <v>2.9142354469616012</v>
+        <v>2.9019406378202612</v>
       </c>
     </row>
     <row r="4">
@@ -227,19 +227,19 @@
         <v>2</v>
       </c>
       <c r="C4" t="n">
-        <v>17.151109449900094</v>
+        <v>17.151109363333543</v>
       </c>
       <c r="D4" t="n">
-        <v>11.901622850629742</v>
+        <v>11.743562965346989</v>
       </c>
       <c r="E4" t="n">
-        <v>5.5610248995158065</v>
+        <v>5.4490341586327409</v>
       </c>
       <c r="F4" t="n">
-        <v>1.2950753683701337</v>
+        <v>1.2699324907637459</v>
       </c>
       <c r="G4" t="n">
-        <v>2.9268205615760818</v>
+        <v>2.9144754269671007</v>
       </c>
     </row>
     <row r="5">
@@ -250,19 +250,19 @@
         <v>3</v>
       </c>
       <c r="C5" t="n">
-        <v>16.295424862284747</v>
+        <v>16.295424742282549</v>
       </c>
       <c r="D5" t="n">
-        <v>12.560481876999509</v>
+        <v>12.582606309838033</v>
       </c>
       <c r="E5" t="n">
-        <v>5.9083360732188019</v>
+        <v>5.8851309686844848</v>
       </c>
       <c r="F5" t="n">
-        <v>1.3708990096289033</v>
+        <v>1.3673061404396027</v>
       </c>
       <c r="G5" t="n">
-        <v>3.0746405377842754</v>
+        <v>3.1044947413340731</v>
       </c>
     </row>
     <row r="6">
@@ -273,19 +273,19 @@
         <v>4</v>
       </c>
       <c r="C6" t="n">
-        <v>15.482551213893149</v>
+        <v>15.482557195990475</v>
       </c>
       <c r="D6" t="n">
-        <v>13.251298457741187</v>
+        <v>13.458460965718087</v>
       </c>
       <c r="E6" t="n">
-        <v>6.2730715843822686</v>
+        <v>6.341652292409159</v>
       </c>
       <c r="F6" t="n">
-        <v>1.4505277884901089</v>
+        <v>1.4700145277509356</v>
       </c>
       <c r="G6" t="n">
-        <v>3.2287174511078045</v>
+        <v>3.3008834541264958</v>
       </c>
     </row>
     <row r="7">
@@ -296,19 +296,19 @@
         <v>5</v>
       </c>
       <c r="C7" t="n">
-        <v>14.710350415995178</v>
+        <v>14.710370498518211</v>
       </c>
       <c r="D7" t="n">
-        <v>13.975368774020673</v>
+        <v>14.388774018195214</v>
       </c>
       <c r="E7" t="n">
-        <v>6.6560621702805065</v>
+        <v>6.828120113614907</v>
       </c>
       <c r="F7" t="n">
-        <v>1.5341326347385404</v>
+        <v>1.5794804534796312</v>
       </c>
       <c r="G7" t="n">
-        <v>3.3892375586039121</v>
+        <v>3.5077883898202602</v>
       </c>
     </row>
     <row r="8">
@@ -319,19 +319,19 @@
         <v>6</v>
       </c>
       <c r="C8" t="n">
-        <v>13.976793009901284</v>
+        <v>13.976834316909406</v>
       </c>
       <c r="D8" t="n">
-        <v>14.734031361407453</v>
+        <v>15.376520574247115</v>
       </c>
       <c r="E8" t="n">
-        <v>7.0581777586401691</v>
+        <v>7.3464273852942981</v>
       </c>
       <c r="F8" t="n">
-        <v>1.62189009509744</v>
+        <v>1.6961058826427065</v>
       </c>
       <c r="G8" t="n">
-        <v>3.5563936163084455</v>
+        <v>3.7256361848276147</v>
       </c>
     </row>
     <row r="9">
@@ -342,19 +342,19 @@
         <v>7</v>
       </c>
       <c r="C9" t="n">
-        <v>13.279949761860857</v>
+        <v>13.280017732025962</v>
       </c>
       <c r="D9" t="n">
-        <v>15.507011218950502</v>
+        <v>16.424823372087065</v>
       </c>
       <c r="E9" t="n">
-        <v>7.4667110457393786</v>
+        <v>7.8985579793959166</v>
       </c>
       <c r="F9" t="n">
-        <v>1.7126788486193767</v>
+        <v>1.8203147809853313</v>
       </c>
       <c r="G9" t="n">
-        <v>3.7261716386682044</v>
+        <v>3.9548673621979509</v>
       </c>
     </row>
     <row r="10">
@@ -365,19 +365,19 @@
         <v>8</v>
       </c>
       <c r="C10" t="n">
-        <v>12.6179857323869</v>
+        <v>12.618084976191904</v>
       </c>
       <c r="D10" t="n">
-        <v>16.315431668739294</v>
+        <v>17.512950998868504</v>
       </c>
       <c r="E10" t="n">
-        <v>7.8950948843474409</v>
+        <v>8.4718537136281817</v>
       </c>
       <c r="F10" t="n">
-        <v>1.8078365577061368</v>
+        <v>1.9510450731184761</v>
       </c>
       <c r="G10" t="n">
-        <v>3.9025385292929129</v>
+        <v>4.1911020195017992</v>
       </c>
     </row>
     <row r="11">
@@ -388,19 +388,19 @@
         <v>9</v>
       </c>
       <c r="C11" t="n">
-        <v>11.989157848177165</v>
+        <v>11.989294037360672</v>
       </c>
       <c r="D11" t="n">
-        <v>17.160650000574872</v>
+        <v>18.665653761775303</v>
       </c>
       <c r="E11" t="n">
-        <v>8.3442281625796237</v>
+        <v>9.081860554914801</v>
       </c>
       <c r="F11" t="n">
-        <v>1.9075421844730234</v>
+        <v>2.0900360841084065</v>
       </c>
       <c r="G11" t="n">
-        <v>4.0856647799932135</v>
+        <v>4.438979749803452</v>
       </c>
     </row>
     <row r="12">
@@ -411,19 +411,19 @@
         <v>10</v>
       </c>
       <c r="C12" t="n">
-        <v>11.391811234248657</v>
+        <v>11.391991926195143</v>
       </c>
       <c r="D12" t="n">
-        <v>18.044059664095819</v>
+        <v>19.886344394241906</v>
       </c>
       <c r="E12" t="n">
-        <v>8.815047058383719</v>
+        <v>9.7306928491115894</v>
       </c>
       <c r="F12" t="n">
-        <v>2.0119750698300853</v>
+        <v>2.2377510857091494</v>
       </c>
       <c r="G12" t="n">
-        <v>4.2757212660598505</v>
+        <v>4.698908593669235</v>
       </c>
     </row>
     <row r="13">
@@ -434,19 +434,19 @@
         <v>11</v>
       </c>
       <c r="C13" t="n">
-        <v>10.824375653840216</v>
+        <v>10.824629304986523</v>
       </c>
       <c r="D13" t="n">
-        <v>18.967119711938075</v>
+        <v>21.178747432859097</v>
       </c>
       <c r="E13" t="n">
-        <v>9.3084592131987574</v>
+        <v>10.419898568801266</v>
       </c>
       <c r="F13" t="n">
-        <v>2.1213302915881358</v>
+        <v>2.394680345697183</v>
       </c>
       <c r="G13" t="n">
-        <v>4.4728775209844214</v>
+        <v>4.971271581065805</v>
       </c>
     </row>
     <row r="14">
@@ -457,19 +457,19 @@
         <v>12</v>
       </c>
       <c r="C14" t="n">
-        <v>10.285369954255879</v>
+        <v>10.285824079004511</v>
       </c>
       <c r="D14" t="n">
-        <v>19.907753383468645</v>
+        <v>22.533112725589366</v>
       </c>
       <c r="E14" t="n">
-        <v>9.8124742339280822</v>
+        <v>10.993972989219792</v>
       </c>
       <c r="F14" t="n">
-        <v>2.2340784359249288</v>
+        <v>2.5545482455772817</v>
       </c>
       <c r="G14" t="n">
-        <v>4.6713731786429609</v>
+        <v>5.2426774236444409</v>
       </c>
     </row>
     <row r="15">
@@ -480,19 +480,19 @@
         <v>13</v>
       </c>
       <c r="C15" t="n">
-        <v>9.773458558879307</v>
+        <v>9.7885761720869606</v>
       </c>
       <c r="D15" t="n">
-        <v>20.903489930931595</v>
+        <v>23.907380808444643</v>
       </c>
       <c r="E15" t="n">
-        <v>10.273496093673483</v>
+        <v>11.599119170688397</v>
       </c>
       <c r="F15" t="n">
-        <v>2.3521361764002728</v>
+        <v>2.7193137002978527</v>
       </c>
       <c r="G15" t="n">
-        <v>4.873699902249963</v>
+        <v>5.5164279101095817</v>
       </c>
     </row>
     <row r="16">
@@ -503,19 +503,19 @@
         <v>14</v>
       </c>
       <c r="C16" t="n">
-        <v>9.2945258250311227</v>
+        <v>9.3288524831180677</v>
       </c>
       <c r="D16" t="n">
-        <v>21.966228537748787</v>
+        <v>25.29108096281827</v>
       </c>
       <c r="E16" t="n">
-        <v>10.709493157473492</v>
+        <v>12.256991480450933</v>
       </c>
       <c r="F16" t="n">
-        <v>2.4760000087520164</v>
+        <v>2.887166263721979</v>
       </c>
       <c r="G16" t="n">
-        <v>5.0839029394763244</v>
+        <v>5.7941464269579672</v>
       </c>
     </row>
     <row r="17">
@@ -526,19 +526,19 @@
         <v>15</v>
       </c>
       <c r="C17" t="n">
-        <v>8.8528254855625335</v>
+        <v>8.9002882341555356</v>
       </c>
       <c r="D17" t="n">
-        <v>23.028810053030384</v>
+        <v>26.693663819101396</v>
       </c>
       <c r="E17" t="n">
-        <v>11.197624225643779</v>
+        <v>12.937235828002239</v>
       </c>
       <c r="F17" t="n">
-        <v>2.6029837560238955</v>
+        <v>3.0621924915614662</v>
       </c>
       <c r="G17" t="n">
-        <v>5.2971471475548411</v>
+        <v>6.0788879025416493</v>
       </c>
     </row>
     <row r="18">
@@ -549,19 +549,19 @@
         <v>16</v>
       </c>
       <c r="C18" t="n">
-        <v>8.4412706401271365</v>
+        <v>8.4994453125985885</v>
       </c>
       <c r="D18" t="n">
-        <v>24.146832526797667</v>
+        <v>28.135579462098786</v>
       </c>
       <c r="E18" t="n">
-        <v>11.740839982303012</v>
+        <v>13.663348411852137</v>
       </c>
       <c r="F18" t="n">
-        <v>2.7366434147396008</v>
+        <v>3.2347009704496545</v>
       </c>
       <c r="G18" t="n">
-        <v>5.5220777593793695</v>
+        <v>6.3697617258067023</v>
       </c>
     </row>
     <row r="19">
@@ -572,19 +572,19 @@
         <v>17</v>
       </c>
       <c r="C19" t="n">
-        <v>8.056178463919105</v>
+        <v>8.1236576459036094</v>
       </c>
       <c r="D19" t="n">
-        <v>25.32062691033029</v>
+        <v>29.629046615381903</v>
       </c>
       <c r="E19" t="n">
-        <v>12.328280082356207</v>
+        <v>14.431514699335368</v>
       </c>
       <c r="F19" t="n">
-        <v>2.8770149887573782</v>
+        <v>3.4124466403202391</v>
       </c>
       <c r="G19" t="n">
-        <v>5.7577134023550798</v>
+        <v>6.6695211279856776</v>
       </c>
     </row>
     <row r="20">
@@ -595,19 +595,19 @@
         <v>18</v>
       </c>
       <c r="C20" t="n">
-        <v>7.6951356551891639</v>
+        <v>7.770844777259394</v>
       </c>
       <c r="D20" t="n">
-        <v>26.550671100153405</v>
+        <v>31.150155176189351</v>
       </c>
       <c r="E20" t="n">
-        <v>12.956501454754438</v>
+        <v>15.229290243809551</v>
       </c>
       <c r="F20" t="n">
-        <v>3.0242111644217862</v>
+        <v>3.595311365599053</v>
       </c>
       <c r="G20" t="n">
-        <v>6.003677167568596</v>
+        <v>6.9694473957520566</v>
       </c>
     </row>
     <row r="21">
@@ -618,19 +618,19 @@
         <v>19</v>
       </c>
       <c r="C21" t="n">
-        <v>7.3562288326362024</v>
+        <v>7.4391876259265839</v>
       </c>
       <c r="D21" t="n">
-        <v>27.837719511442142</v>
+        <v>32.634599474456557</v>
       </c>
       <c r="E21" t="n">
-        <v>13.623519231115377</v>
+        <v>16.006069718117502</v>
       </c>
       <c r="F21" t="n">
-        <v>3.1783655824993553</v>
+        <v>3.7685098323746193</v>
       </c>
       <c r="G21" t="n">
-        <v>6.2597456555673787</v>
+        <v>7.2667680600129625</v>
       </c>
     </row>
     <row r="22">
@@ -641,19 +641,19 @@
         <v>20</v>
       </c>
       <c r="C22" t="n">
-        <v>7.0378837981678748</v>
+        <v>7.1271913252154731</v>
       </c>
       <c r="D22" t="n">
-        <v>29.126108851969484</v>
+        <v>34.143602665747039</v>
       </c>
       <c r="E22" t="n">
-        <v>14.295876490471489</v>
+        <v>16.739851401149537</v>
       </c>
       <c r="F22" t="n">
-        <v>3.3296820229875168</v>
+        <v>3.9453078231287528</v>
       </c>
       <c r="G22" t="n">
-        <v>6.5172421977493329</v>
+        <v>7.5614615992243959</v>
       </c>
     </row>
     <row r="23">
@@ -664,19 +664,19 @@
         <v>21</v>
       </c>
       <c r="C23" t="n">
-        <v>6.7385670173232297</v>
+        <v>6.839300961566714</v>
       </c>
       <c r="D23" t="n">
-        <v>30.468125506528292</v>
+        <v>35.655501349480105</v>
       </c>
       <c r="E23" t="n">
-        <v>15.001279893158044</v>
+        <v>17.451099588143133</v>
       </c>
       <c r="F23" t="n">
-        <v>3.4872218085105482</v>
+        <v>4.1212799325602809</v>
       </c>
       <c r="G23" t="n">
-        <v>6.7839259102697937</v>
+        <v>7.852660122207026</v>
       </c>
     </row>
     <row r="24">
@@ -687,19 +687,19 @@
         <v>22</v>
       </c>
       <c r="C24" t="n">
-        <v>6.4572233460600739</v>
+        <v>6.5764486819069194</v>
       </c>
       <c r="D24" t="n">
-        <v>31.833894663233249</v>
+        <v>37.122617633672654</v>
       </c>
       <c r="E24" t="n">
-        <v>15.651626175453462</v>
+        <v>18.174463986106474</v>
       </c>
       <c r="F24" t="n">
-        <v>3.647259856196476</v>
+        <v>4.2984230028609893</v>
       </c>
       <c r="G24" t="n">
-        <v>7.0498717568838165</v>
+        <v>8.1363834491797924</v>
       </c>
     </row>
     <row r="25">
@@ -710,19 +710,19 @@
         <v>23</v>
       </c>
       <c r="C25" t="n">
-        <v>6.1989609565381638</v>
+        <v>6.3339409184765607</v>
       </c>
       <c r="D25" t="n">
-        <v>33.202018483510933</v>
+        <v>38.593956034831628</v>
       </c>
       <c r="E25" t="n">
-        <v>16.302987854059133</v>
+        <v>18.916028753580395</v>
       </c>
       <c r="F25" t="n">
-        <v>3.8071167093579139</v>
+        <v>4.4798151082749609</v>
       </c>
       <c r="G25" t="n">
-        <v>7.3124011435552898</v>
+        <v>8.423435608940002</v>
       </c>
     </row>
     <row r="26">
@@ -733,19 +733,19 @@
         <v>24</v>
       </c>
       <c r="C26" t="n">
-        <v>5.9629408487635516</v>
+        <v>6.1089820731559312</v>
       </c>
       <c r="D26" t="n">
-        <v>34.517602616117244</v>
+        <v>40.104434854747367</v>
       </c>
       <c r="E26" t="n">
-        <v>16.947876931654065</v>
+        <v>19.690502490974268</v>
       </c>
       <c r="F26" t="n">
-        <v>3.9683339696014883</v>
+        <v>4.6647346670925858</v>
       </c>
       <c r="G26" t="n">
-        <v>7.5693160633801835</v>
+        <v>8.7174234847896237</v>
       </c>
     </row>
     <row r="27">
@@ -756,19 +756,19 @@
         <v>25</v>
       </c>
       <c r="C27" t="n">
-        <v>5.7450858367637272</v>
+        <v>5.8999876938457589</v>
       </c>
       <c r="D27" t="n">
-        <v>35.87153955397357</v>
+        <v>41.580466093822665</v>
       </c>
       <c r="E27" t="n">
-        <v>17.632815844250199</v>
+        <v>20.470618213818288</v>
       </c>
       <c r="F27" t="n">
-        <v>4.1332802539170244</v>
+        <v>4.8359586376311867</v>
       </c>
       <c r="G27" t="n">
-        <v>7.833986251743589</v>
+        <v>9.0046523774877194</v>
       </c>
     </row>
     <row r="28">
@@ -779,19 +779,19 @@
         <v>26</v>
       </c>
       <c r="C28" t="n">
-        <v>5.543078914399052</v>
+        <v>5.7050400407172122</v>
       </c>
       <c r="D28" t="n">
-        <v>37.249008033945067</v>
+        <v>43.037409338940648</v>
       </c>
       <c r="E28" t="n">
-        <v>18.343222187584637</v>
+        <v>21.254263293653942</v>
       </c>
       <c r="F28" t="n">
-        <v>4.2999843354021943</v>
+        <v>5.0044978233858393</v>
       </c>
       <c r="G28" t="n">
-        <v>8.1030057864697937</v>
+        <v>9.2832502040331981</v>
       </c>
     </row>
     <row r="29">
@@ -802,19 +802,19 @@
         <v>27</v>
       </c>
       <c r="C29" t="n">
-        <v>5.3553476934278077</v>
+        <v>5.5228406307524596</v>
       </c>
       <c r="D29" t="n">
-        <v>38.590755326461043</v>
+        <v>44.487493510247553</v>
       </c>
       <c r="E29" t="n">
-        <v>19.047016449960694</v>
+        <v>22.030126730417624</v>
       </c>
       <c r="F29" t="n">
-        <v>4.453281518436742</v>
+        <v>5.1708606107779209</v>
       </c>
       <c r="G29" t="n">
-        <v>8.3690036821629246</v>
+        <v>9.564446076646826</v>
       </c>
     </row>
     <row r="30">
@@ -825,19 +825,19 @@
         <v>28</v>
       </c>
       <c r="C30" t="n">
-        <v>5.1803431671358648</v>
+        <v>5.3526517079782874</v>
       </c>
       <c r="D30" t="n">
-        <v>39.911866328324315</v>
+        <v>45.962101988258468</v>
       </c>
       <c r="E30" t="n">
-        <v>19.752597386715777</v>
+        <v>22.8016249185197</v>
       </c>
       <c r="F30" t="n">
-        <v>4.6037390608653244</v>
+        <v>5.3404601862890448</v>
       </c>
       <c r="G30" t="n">
-        <v>8.6264018762727108</v>
+        <v>9.8460605776265542</v>
       </c>
     </row>
     <row r="31">
@@ -848,19 +848,19 @@
         <v>29</v>
       </c>
       <c r="C31" t="n">
-        <v>5.0168650495352543</v>
+        <v>5.1962715428129114</v>
       </c>
       <c r="D31" t="n">
-        <v>41.273003452851114</v>
+        <v>47.519812752694349</v>
       </c>
       <c r="E31" t="n">
-        <v>20.47083081052768</v>
+        <v>23.574233312299391</v>
       </c>
       <c r="F31" t="n">
-        <v>4.7581366820397584</v>
+        <v>5.5215259202434783</v>
       </c>
       <c r="G31" t="n">
-        <v>8.8895802996994835</v>
+        <v>10.140782367075341</v>
       </c>
     </row>
     <row r="32">
@@ -871,19 +871,19 @@
         <v>30</v>
       </c>
       <c r="C32" t="n">
-        <v>4.8654458277538035</v>
+        <v>5.0563350067320316</v>
       </c>
       <c r="D32" t="n">
-        <v>42.648947539311784</v>
+        <v>49.072243881297865</v>
       </c>
       <c r="E32" t="n">
-        <v>21.169526726261076</v>
+        <v>24.287852208147573</v>
       </c>
       <c r="F32" t="n">
-        <v>4.9165879604486662</v>
+        <v>5.6986903723230178</v>
       </c>
       <c r="G32" t="n">
-        <v>9.152276005743591</v>
+        <v>10.422400324076703</v>
       </c>
     </row>
     <row r="33">
@@ -894,19 +894,19 @@
         <v>31</v>
       </c>
       <c r="C33" t="n">
-        <v>4.7283376994820658</v>
+        <v>4.9382776877661927</v>
       </c>
       <c r="D33" t="n">
-        <v>44.076650880764745</v>
+        <v>50.425426723780475</v>
       </c>
       <c r="E33" t="n">
-        <v>21.858440743425032</v>
+        <v>24.936624828056914</v>
       </c>
       <c r="F33" t="n">
-        <v>5.0756575208230048</v>
+        <v>5.8350725820032938</v>
       </c>
       <c r="G33" t="n">
-        <v>9.4219016401291338</v>
+        <v>10.677221725290172</v>
       </c>
     </row>
     <row r="34">
@@ -917,19 +917,19 @@
         <v>32</v>
       </c>
       <c r="C34" t="n">
-        <v>4.6080798336602253</v>
+        <v>4.836561323191126</v>
       </c>
       <c r="D34" t="n">
-        <v>45.41177280139253</v>
+        <v>51.798699292026434</v>
       </c>
       <c r="E34" t="n">
-        <v>22.478390201215063</v>
+        <v>25.578241261831298</v>
       </c>
       <c r="F34" t="n">
-        <v>5.2149423402916906</v>
+        <v>5.9749954050213434</v>
       </c>
       <c r="G34" t="n">
-        <v>9.6704169932276098</v>
+        <v>10.932532548489126</v>
       </c>
     </row>
     <row r="35">
@@ -940,19 +940,19 @@
         <v>33</v>
       </c>
       <c r="C35" t="n">
-        <v>4.5062682626085824</v>
+        <v>4.7520605409928738</v>
       </c>
       <c r="D35" t="n">
-        <v>46.639176719172433</v>
+        <v>53.15645235495554</v>
       </c>
       <c r="E35" t="n">
-        <v>23.05882524912704</v>
+        <v>26.211263015803944</v>
       </c>
       <c r="F35" t="n">
-        <v>5.3383092139784214</v>
+        <v>6.1178115488565723</v>
       </c>
       <c r="G35" t="n">
-        <v>9.9017681486643845</v>
+        <v>11.190250303200189</v>
       </c>
     </row>
     <row r="36">
@@ -963,19 +963,19 @@
         <v>34</v>
       </c>
       <c r="C36" t="n">
-        <v>4.4197684077452024</v>
+        <v>4.6830301050829064</v>
       </c>
       <c r="D36" t="n">
-        <v>47.887005501952054</v>
+        <v>54.52676198853267</v>
       </c>
       <c r="E36" t="n">
-        <v>23.651240821064484</v>
+        <v>26.831621419112214</v>
       </c>
       <c r="F36" t="n">
-        <v>5.4675298950600899</v>
+        <v>6.2665498170438934</v>
       </c>
       <c r="G36" t="n">
-        <v>10.1393658262031</v>
+        <v>11.454223352117696</v>
       </c>
     </row>
     <row r="37">
@@ -986,19 +986,19 @@
         <v>35</v>
       </c>
       <c r="C37" t="n">
-        <v>4.3472720522040396</v>
+        <v>4.6293356096596598</v>
       </c>
       <c r="D37" t="n">
-        <v>49.155280554319582</v>
+        <v>55.856139239386437</v>
       </c>
       <c r="E37" t="n">
-        <v>24.234599290650856</v>
+        <v>27.418625432448874</v>
       </c>
       <c r="F37" t="n">
-        <v>5.6007521126658073</v>
+        <v>6.4191660034698339</v>
       </c>
       <c r="G37" t="n">
-        <v>10.381606445171144</v>
+        <v>11.719759276702145</v>
       </c>
     </row>
     <row r="38">
@@ -1009,19 +1009,19 @@
         <v>36</v>
       </c>
       <c r="C38" t="n">
-        <v>4.2895204682691412</v>
+        <v>4.5891582128270363</v>
       </c>
       <c r="D38" t="n">
-        <v>50.395788529813082</v>
+        <v>57.187860712153018</v>
       </c>
       <c r="E38" t="n">
-        <v>24.774691381844296</v>
+        <v>27.985916886367363</v>
       </c>
       <c r="F38" t="n">
-        <v>5.7383570132849178</v>
+        <v>6.5753359038708412</v>
       </c>
       <c r="G38" t="n">
-        <v>10.627465328778921</v>
+        <v>11.988114368647929</v>
       </c>
     </row>
     <row r="39">
@@ -1032,19 +1032,19 @@
         <v>37</v>
       </c>
       <c r="C39" t="n">
-        <v>4.246170840527034</v>
+        <v>4.5629953968301411</v>
       </c>
       <c r="D39" t="n">
-        <v>51.593770957025072</v>
+        <v>58.493217293364246</v>
       </c>
       <c r="E39" t="n">
-        <v>25.288315686750682</v>
+        <v>28.576819002757134</v>
       </c>
       <c r="F39" t="n">
-        <v>5.8784483845503432</v>
+        <v>6.7326787971295818</v>
       </c>
       <c r="G39" t="n">
-        <v>10.872201540144458</v>
+        <v>12.253294152812428</v>
       </c>
     </row>
     <row r="40">
@@ -1055,19 +1055,19 @@
         <v>38</v>
       </c>
       <c r="C40" t="n">
-        <v>4.215329530189841</v>
+        <v>4.5467660816275997</v>
       </c>
       <c r="D40" t="n">
-        <v>52.802906480376798</v>
+        <v>59.840687523643901</v>
       </c>
       <c r="E40" t="n">
-        <v>25.813167367966461</v>
+        <v>29.19327345027077</v>
       </c>
       <c r="F40" t="n">
-        <v>6.0210503150236487</v>
+        <v>6.8947692711139617</v>
       </c>
       <c r="G40" t="n">
-        <v>11.118534731521649</v>
+        <v>12.526673288983034</v>
       </c>
     </row>
     <row r="41">
@@ -1078,19 +1078,19 @@
         <v>39</v>
       </c>
       <c r="C41" t="n">
-        <v>4.196037428472402</v>
+        <v>4.5397456894133299</v>
       </c>
       <c r="D41" t="n">
-        <v>54.018561163775296</v>
+        <v>61.202053372970099</v>
       </c>
       <c r="E41" t="n">
-        <v>26.368311050461021</v>
+        <v>29.780169739480293</v>
       </c>
       <c r="F41" t="n">
-        <v>6.1667391963872191</v>
+        <v>7.057426519537513</v>
       </c>
       <c r="G41" t="n">
-        <v>11.36734825921207</v>
+        <v>12.798507209543011</v>
       </c>
     </row>
     <row r="42">
@@ -1101,19 +1101,19 @@
         <v>40</v>
       </c>
       <c r="C42" t="n">
-        <v>4.1853309063673212</v>
+        <v>4.5446909832637647</v>
       </c>
       <c r="D42" t="n">
-        <v>55.280836376915083</v>
+        <v>62.53667960855298</v>
       </c>
       <c r="E42" t="n">
-        <v>26.916813871789021</v>
+        <v>30.360896930493645</v>
       </c>
       <c r="F42" t="n">
-        <v>6.3158783112968164</v>
+        <v>7.2156684900596204</v>
       </c>
       <c r="G42" t="n">
-        <v>11.623402559303765</v>
+        <v>13.064996232811882</v>
       </c>
     </row>
     <row r="43">
@@ -1124,19 +1124,19 @@
         <v>41</v>
       </c>
       <c r="C43" t="n">
-        <v>4.1855670140231078</v>
+        <v>4.5606490201879355</v>
       </c>
       <c r="D43" t="n">
-        <v>56.525361047923312</v>
+        <v>63.785751283585391</v>
       </c>
       <c r="E43" t="n">
-        <v>27.450470478145309</v>
+        <v>30.917507343061491</v>
       </c>
       <c r="F43" t="n">
-        <v>6.4641417057217057</v>
+        <v>7.3596375696933807</v>
       </c>
       <c r="G43" t="n">
-        <v>11.873043176076697</v>
+        <v>13.322223127795771</v>
       </c>
     </row>
     <row r="44">
@@ -1147,19 +1147,19 @@
         <v>42</v>
       </c>
       <c r="C44" t="n">
-        <v>4.1967040144134415</v>
+        <v>4.5846095163806915</v>
       </c>
       <c r="D44" t="n">
-        <v>57.694735127628185</v>
+        <v>65.045196772423168</v>
       </c>
       <c r="E44" t="n">
-        <v>27.968717230654708</v>
+        <v>31.452599870516721</v>
       </c>
       <c r="F44" t="n">
-        <v>6.5994507570656955</v>
+        <v>7.5064310717978886</v>
       </c>
       <c r="G44" t="n">
-        <v>12.112142114938891</v>
+        <v>13.581418449464524</v>
       </c>
     </row>
     <row r="45">
@@ -1170,19 +1170,19 @@
         <v>43</v>
       </c>
       <c r="C45" t="n">
-        <v>4.2162751969547996</v>
+        <v>4.6184752217465714</v>
       </c>
       <c r="D45" t="n">
-        <v>58.831382784076503</v>
+        <v>66.250749249526905</v>
       </c>
       <c r="E45" t="n">
-        <v>28.470990236010074</v>
+        <v>31.935498039049097</v>
       </c>
       <c r="F45" t="n">
-        <v>6.7326002779112795</v>
+        <v>7.6414436225416669</v>
       </c>
       <c r="G45" t="n">
-        <v>12.348819397301437</v>
+        <v>13.843243217946396</v>
       </c>
     </row>
     <row r="46">
@@ -1193,19 +1193,19 @@
         <v>44</v>
       </c>
       <c r="C46" t="n">
-        <v>4.2429367093571351</v>
+        <v>4.6624080259105378</v>
       </c>
       <c r="D46" t="n">
-        <v>59.965353396539314</v>
+        <v>67.403023353027379</v>
       </c>
       <c r="E46" t="n">
-        <v>28.918985720673373</v>
+        <v>32.429034948155341</v>
       </c>
       <c r="F46" t="n">
-        <v>6.8596388270370223</v>
+        <v>7.7716615325922831</v>
       </c>
       <c r="G46" t="n">
-        <v>12.58960118814935</v>
+        <v>14.098363268343013</v>
       </c>
     </row>
     <row r="47">
@@ -1216,19 +1216,19 @@
         <v>45</v>
       </c>
       <c r="C47" t="n">
-        <v>4.2809523417758131</v>
+        <v>4.7118956901290634</v>
       </c>
       <c r="D47" t="n">
-        <v>61.003670384038571</v>
+        <v>68.585070891047707</v>
       </c>
       <c r="E47" t="n">
-        <v>29.352232192514553</v>
+        <v>32.946973165566675</v>
       </c>
       <c r="F47" t="n">
-        <v>6.9750394586475482</v>
+        <v>7.9064199277339355</v>
       </c>
       <c r="G47" t="n">
-        <v>12.821747034013683</v>
+        <v>14.360500604425896</v>
       </c>
     </row>
     <row r="48">
@@ -1239,19 +1239,19 @@
         <v>46</v>
       </c>
       <c r="C48" t="n">
-        <v>4.3250453199170842</v>
+        <v>4.7656759032051257</v>
       </c>
       <c r="D48" t="n">
-        <v>62.070877750929625</v>
+        <v>69.793074987394789</v>
       </c>
       <c r="E48" t="n">
-        <v>29.812628555188745</v>
+        <v>33.482779976649297</v>
       </c>
       <c r="F48" t="n">
-        <v>7.0952994610544513</v>
+        <v>8.0446639907541488</v>
       </c>
       <c r="G48" t="n">
-        <v>13.060615571760993</v>
+        <v>14.628581586245417</v>
       </c>
     </row>
     <row r="49">
@@ -1262,19 +1262,19 @@
         <v>47</v>
       </c>
       <c r="C49" t="n">
-        <v>4.3736363223176919</v>
+        <v>4.8231426597039899</v>
       </c>
       <c r="D49" t="n">
-        <v>63.162790730163294</v>
+        <v>71.026823436225172</v>
       </c>
       <c r="E49" t="n">
-        <v>30.291238740207646</v>
+        <v>34.028494204467606</v>
       </c>
       <c r="F49" t="n">
-        <v>7.2190288767691264</v>
+        <v>8.1858171064186998</v>
       </c>
       <c r="G49" t="n">
-        <v>13.305120956906697</v>
+        <v>14.902232392475101</v>
       </c>
     </row>
     <row r="50">
@@ -1285,19 +1285,19 @@
         <v>48</v>
       </c>
       <c r="C50" t="n">
-        <v>4.4260135904967646</v>
+        <v>4.8843042999787745</v>
       </c>
       <c r="D50" t="n">
-        <v>64.279107048285084</v>
+        <v>72.292808433685551</v>
       </c>
       <c r="E50" t="n">
-        <v>30.779526912264942</v>
+        <v>34.574549462553769</v>
       </c>
       <c r="F50" t="n">
-        <v>7.3455420910990856</v>
+        <v>8.3297098270076244</v>
       </c>
       <c r="G50" t="n">
-        <v>13.55498892958034</v>
+        <v>15.182710386505139</v>
       </c>
     </row>
     <row r="51">
@@ -1308,19 +1308,19 @@
         <v>49</v>
       </c>
       <c r="C51" t="n">
-        <v>4.482112772486456</v>
+        <v>4.9502504176155426</v>
       </c>
       <c r="D51" t="n">
-        <v>65.425792078185722</v>
+        <v>73.426491538349168</v>
       </c>
       <c r="E51" t="n">
-        <v>31.269346935529839</v>
+        <v>35.097737195752138</v>
       </c>
       <c r="F51" t="n">
-        <v>7.4745952482819975</v>
+        <v>8.4639180303445283</v>
       </c>
       <c r="G51" t="n">
-        <v>13.81164187520756</v>
+        <v>15.421466140330184</v>
       </c>
     </row>
     <row r="52">
@@ -1331,19 +1331,19 @@
         <v>50</v>
       </c>
       <c r="C52" t="n">
-        <v>4.5428555510073911</v>
+        <v>5.0181930985297321</v>
       </c>
       <c r="D52" t="n">
-        <v>66.445631887420461</v>
+        <v>74.551452953927381</v>
       </c>
       <c r="E52" t="n">
-        <v>31.749927603373106</v>
+        <v>35.611570621058831</v>
       </c>
       <c r="F52" t="n">
-        <v>7.5953215613517262</v>
+        <v>8.5973584138668127</v>
       </c>
       <c r="G52" t="n">
-        <v>14.028852948707378</v>
+        <v>15.662315030184681</v>
       </c>
     </row>
     <row r="53">
@@ -1354,19 +1354,19 @@
         <v>51</v>
       </c>
       <c r="C53" t="n">
-        <v>4.6043632896067139</v>
+        <v>5.0878619592753553</v>
       </c>
       <c r="D53" t="n">
-        <v>67.50055896062679</v>
+        <v>75.661588090213925</v>
       </c>
       <c r="E53" t="n">
-        <v>32.217784978633738</v>
+        <v>36.118131566130536</v>
       </c>
       <c r="F53" t="n">
-        <v>7.7173367117036369</v>
+        <v>8.7300038691721671</v>
       </c>
       <c r="G53" t="n">
-        <v>14.259792361173544</v>
+        <v>15.903731603678711</v>
       </c>
     </row>
     <row r="54">
@@ -1377,19 +1377,19 @@
         <v>52</v>
       </c>
       <c r="C54" t="n">
-        <v>4.6684774322347415</v>
+        <v>5.1585785915582836</v>
       </c>
       <c r="D54" t="n">
-        <v>68.503564963862061</v>
+        <v>76.787144165726701</v>
       </c>
       <c r="E54" t="n">
-        <v>32.674772600766843</v>
+        <v>36.632793316609266</v>
       </c>
       <c r="F54" t="n">
-        <v>7.8363881419614412</v>
+        <v>8.8642168595084669</v>
       </c>
       <c r="G54" t="n">
-        <v>14.47937217580327</v>
+        <v>16.148385736467841</v>
       </c>
     </row>
     <row r="55">
@@ -1400,19 +1400,19 @@
         <v>53</v>
       </c>
       <c r="C55" t="n">
-        <v>4.7335467096931767</v>
+        <v>5.2303531235516134</v>
       </c>
       <c r="D55" t="n">
-        <v>69.520419153002933</v>
+        <v>77.931382009408125</v>
       </c>
       <c r="E55" t="n">
-        <v>33.138947934352466</v>
+        <v>37.149642402967544</v>
       </c>
       <c r="F55" t="n">
-        <v>7.9567673558874139</v>
+        <v>8.9996389397543233</v>
       </c>
       <c r="G55" t="n">
-        <v>14.701853895417559</v>
+        <v>16.396213400196306</v>
       </c>
     </row>
     <row r="56">
@@ -1423,19 +1423,19 @@
         <v>54</v>
       </c>
       <c r="C56" t="n">
-        <v>4.7996237169323477</v>
+        <v>5.3046853298286205</v>
       </c>
       <c r="D56" t="n">
-        <v>70.554611531410586</v>
+        <v>79.046784144608651</v>
       </c>
       <c r="E56" t="n">
-        <v>33.604837178506052</v>
+        <v>37.661086141759426</v>
       </c>
       <c r="F56" t="n">
-        <v>8.0780929323904918</v>
+        <v>9.1339085088611611</v>
       </c>
       <c r="G56" t="n">
-        <v>14.92746852333207</v>
+        <v>16.635395426495187</v>
       </c>
     </row>
     <row r="57">
@@ -1446,19 +1446,19 @@
         <v>55</v>
       </c>
       <c r="C57" t="n">
-        <v>4.8681294372010191</v>
+        <v>5.3803010925237205</v>
       </c>
       <c r="D57" t="n">
-        <v>71.562028286614449</v>
+        <v>80.17718542334687</v>
       </c>
       <c r="E57" t="n">
-        <v>34.067180736399287</v>
+        <v>38.179781632086417</v>
       </c>
       <c r="F57" t="n">
-        <v>8.1984472159965378</v>
+        <v>9.269959092047678</v>
       </c>
       <c r="G57" t="n">
-        <v>15.144868477835061</v>
+        <v>16.878357185078077</v>
       </c>
     </row>
     <row r="58">
@@ -1469,19 +1469,19 @@
         <v>56</v>
       </c>
       <c r="C58" t="n">
-        <v>4.9377205099100143</v>
+        <v>5.4568218835981961</v>
       </c>
       <c r="D58" t="n">
-        <v>72.582400788785534</v>
+        <v>81.321591427323767</v>
       </c>
       <c r="E58" t="n">
-        <v>34.535634153886264</v>
+        <v>38.704443934713161</v>
       </c>
       <c r="F58" t="n">
-        <v>8.3203378048878722</v>
+        <v>9.4076632514340162</v>
       </c>
       <c r="G58" t="n">
-        <v>15.365527669067076</v>
+        <v>17.124468628586087</v>
       </c>
     </row>
     <row r="59">
@@ -1492,19 +1492,19 @@
         <v>57</v>
       </c>
       <c r="C59" t="n">
-        <v>5.0080752615130759</v>
+        <v>5.5342066335783331</v>
       </c>
       <c r="D59" t="n">
-        <v>73.615070850487299</v>
+        <v>82.479924768638327</v>
       </c>
       <c r="E59" t="n">
-        <v>35.009153132322616</v>
+        <v>39.234920085332909</v>
       </c>
       <c r="F59" t="n">
-        <v>8.4436522041943771</v>
+        <v>9.5470404249756946</v>
       </c>
       <c r="G59" t="n">
-        <v>15.588961465074402</v>
+        <v>17.373631272325323</v>
       </c>
     </row>
     <row r="60">
@@ -1515,19 +1515,19 @@
         <v>58</v>
       </c>
       <c r="C60" t="n">
-        <v>5.0791748123354736</v>
+        <v>5.6124696477795917</v>
       </c>
       <c r="D60" t="n">
-        <v>74.66005210222859</v>
+        <v>83.652302502227656</v>
       </c>
       <c r="E60" t="n">
-        <v>35.487677296594477</v>
+        <v>39.771266746980203</v>
       </c>
       <c r="F60" t="n">
-        <v>8.5684175593648408</v>
+        <v>9.6881294938687077</v>
       </c>
       <c r="G60" t="n">
-        <v>15.815107611409186</v>
+        <v>17.625840849061259</v>
       </c>
     </row>
     <row r="61">
@@ -1538,19 +1538,19 @@
         <v>59</v>
       </c>
       <c r="C61" t="n">
-        <v>5.151045687274328</v>
+        <v>5.6916419398113343</v>
       </c>
       <c r="D61" t="n">
-        <v>75.717500341858553</v>
+        <v>84.838915981665906</v>
       </c>
       <c r="E61" t="n">
-        <v>35.971306802370336</v>
+        <v>40.313596856157403</v>
       </c>
       <c r="F61" t="n">
-        <v>8.6946768717492411</v>
+        <v>9.8309719387590135</v>
       </c>
       <c r="G61" t="n">
-        <v>16.043977344227546</v>
+        <v>17.881128154089918</v>
       </c>
     </row>
     <row r="62">
@@ -1561,19 +1561,19 @@
         <v>60</v>
       </c>
       <c r="C62" t="n">
-        <v>5.22372559848771</v>
+        <v>5.771758889483837</v>
       </c>
       <c r="D62" t="n">
-        <v>76.78761867063497</v>
+        <v>86.039982558484184</v>
       </c>
       <c r="E62" t="n">
-        <v>36.460176580249353</v>
+        <v>40.862048640358644</v>
       </c>
       <c r="F62" t="n">
-        <v>8.8224732422045058</v>
+        <v>9.9756088948796808</v>
       </c>
       <c r="G62" t="n">
-        <v>16.275606904299721</v>
+        <v>18.13953833730039</v>
       </c>
     </row>
     <row r="63">
@@ -1584,19 +1584,19 @@
         <v>61</v>
       </c>
       <c r="C63" t="n">
-        <v>5.2972538205930855</v>
+        <v>5.8528547070164025</v>
       </c>
       <c r="D63" t="n">
-        <v>77.870622487406393</v>
+        <v>87.255731441018057</v>
       </c>
       <c r="E63" t="n">
-        <v>36.954438831727188</v>
+        <v>41.416756929870473</v>
       </c>
       <c r="F63" t="n">
-        <v>8.9518482484791644</v>
+        <v>10.122078961960366</v>
       </c>
       <c r="G63" t="n">
-        <v>16.51004240392658</v>
+        <v>18.401122099911088</v>
       </c>
     </row>
     <row r="64">
@@ -1607,19 +1607,19 @@
         <v>62</v>
       </c>
       <c r="C64" t="n">
-        <v>5.3716665788472682</v>
+        <v>5.9349617679806697</v>
       </c>
       <c r="D64" t="n">
-        <v>78.966745978917373</v>
+        <v>88.486440305749085</v>
       </c>
       <c r="E64" t="n">
-        <v>37.45422100529025</v>
+        <v>41.977820589415849</v>
       </c>
       <c r="F64" t="n">
-        <v>9.0828388264441973</v>
+        <v>10.270417767432273</v>
       </c>
       <c r="G64" t="n">
-        <v>16.747335433389171</v>
+        <v>18.665939464037361</v>
       </c>
     </row>
     <row r="65">
@@ -1630,19 +1630,19 @@
         <v>63</v>
       </c>
       <c r="C65" t="n">
-        <v>5.4469991590366353</v>
+        <v>6.018115512270005</v>
       </c>
       <c r="D65" t="n">
-        <v>80.076293965306732</v>
+        <v>89.732516463235726</v>
       </c>
       <c r="E65" t="n">
-        <v>37.959636706282012</v>
+        <v>42.545409332909315</v>
       </c>
       <c r="F65" t="n">
-        <v>9.21548044238655</v>
+        <v>10.420664952304532</v>
       </c>
       <c r="G65" t="n">
-        <v>16.987554524140982</v>
+        <v>18.934084001832264</v>
       </c>
     </row>
     <row r="66">
@@ -1653,19 +1653,19 @@
         <v>64</v>
       </c>
       <c r="C66" t="n">
-        <v>5.5232875077662626</v>
+        <v>6.1023465740660194</v>
       </c>
       <c r="D66" t="n">
-        <v>81.199637628858028</v>
+        <v>90.994288106136324</v>
       </c>
       <c r="E66" t="n">
-        <v>38.470852361438794</v>
+        <v>43.119613072024052</v>
       </c>
       <c r="F66" t="n">
-        <v>9.3498117754983294</v>
+        <v>10.572856261508706</v>
       </c>
       <c r="G66" t="n">
-        <v>17.230785837772981</v>
+        <v>19.205627520881883</v>
       </c>
     </row>
     <row r="67">
@@ -1676,19 +1676,19 @@
         <v>65</v>
       </c>
       <c r="C67" t="n">
-        <v>5.6005618179048415</v>
+        <v>6.1876891778334411</v>
       </c>
       <c r="D67" t="n">
-        <v>82.337142220761677</v>
+        <v>92.272686610945087</v>
       </c>
       <c r="E67" t="n">
-        <v>38.987719960993296</v>
+        <v>43.699671028641617</v>
       </c>
       <c r="F67" t="n">
-        <v>9.4858572148643976</v>
+        <v>10.727008268146237</v>
       </c>
       <c r="G67" t="n">
-        <v>17.477096810454722</v>
+        <v>19.480704490718121</v>
       </c>
     </row>
     <row r="68">
@@ -1699,19 +1699,19 @@
         <v>66</v>
       </c>
       <c r="C68" t="n">
-        <v>5.678880754324358</v>
+        <v>6.2742706944468791</v>
       </c>
       <c r="D68" t="n">
-        <v>83.4912810738969</v>
+        <v>93.573847064574224</v>
       </c>
       <c r="E68" t="n">
-        <v>39.50783306020535</v>
+        <v>44.282010624782885</v>
       </c>
       <c r="F68" t="n">
-        <v>9.623587768594323</v>
+        <v>10.883145606240298</v>
       </c>
       <c r="G68" t="n">
-        <v>17.726872230596499</v>
+        <v>19.76032645430422</v>
       </c>
     </row>
     <row r="69">
@@ -1722,19 +1722,19 @@
         <v>67</v>
       </c>
       <c r="C69" t="n">
-        <v>5.7585690909634613</v>
+        <v>6.3626663550363212</v>
       </c>
       <c r="D69" t="n">
-        <v>84.673929422877947</v>
+        <v>94.862596934695674</v>
       </c>
       <c r="E69" t="n">
-        <v>40.033316133572136</v>
+        <v>44.868302143832238</v>
       </c>
       <c r="F69" t="n">
-        <v>9.7633019222256969</v>
+        <v>11.040518575711204</v>
       </c>
       <c r="G69" t="n">
-        <v>17.982806802409506</v>
+        <v>20.038190238652685</v>
       </c>
     </row>
     <row r="70">
@@ -1745,19 +1745,19 @@
         <v>68</v>
       </c>
       <c r="C70" t="n">
-        <v>5.8400592572311165</v>
+        <v>6.4522206624843257</v>
       </c>
       <c r="D70" t="n">
-        <v>85.841838905749469</v>
+        <v>96.178334530566232</v>
       </c>
       <c r="E70" t="n">
-        <v>40.563923458708025</v>
+        <v>45.464638689621886</v>
       </c>
       <c r="F70" t="n">
-        <v>9.9041846629290209</v>
+        <v>11.200129835948403</v>
       </c>
       <c r="G70" t="n">
-        <v>18.236364226885222</v>
+        <v>20.322064285555022</v>
       </c>
     </row>
     <row r="71">
@@ -1768,19 +1768,19 @@
         <v>69</v>
       </c>
       <c r="C71" t="n">
-        <v>5.9225354437432687</v>
+        <v>6.542985017364499</v>
       </c>
       <c r="D71" t="n">
-        <v>87.029141582669808</v>
+        <v>97.511903992107705</v>
       </c>
       <c r="E71" t="n">
-        <v>41.101963319212409</v>
+        <v>46.068898042849312</v>
       </c>
       <c r="F71" t="n">
-        <v>10.04695416612965</v>
+        <v>11.361909838430341</v>
       </c>
       <c r="G71" t="n">
-        <v>18.494249110373119</v>
+        <v>20.609869155672222</v>
       </c>
     </row>
     <row r="72">
@@ -1791,19 +1791,19 @@
         <v>70</v>
       </c>
       <c r="C72" t="n">
-        <v>6.0060467447899235</v>
+        <v>6.6349478730839504</v>
       </c>
       <c r="D72" t="n">
-        <v>88.231915764091937</v>
+        <v>98.862798332758985</v>
       </c>
       <c r="E72" t="n">
-        <v>41.646736154497646</v>
+        <v>46.680885209183536</v>
       </c>
       <c r="F72" t="n">
-        <v>10.191603500163893</v>
+        <v>11.525860935867458</v>
       </c>
       <c r="G72" t="n">
-        <v>18.755552535351821</v>
+        <v>20.901481057470225</v>
       </c>
     </row>
     <row r="73">
@@ -1814,19 +1814,19 @@
         <v>71</v>
       </c>
       <c r="C73" t="n">
-        <v>6.0906006986212944</v>
+        <v>6.7281033299122575</v>
       </c>
       <c r="D73" t="n">
-        <v>89.450034368491586</v>
+        <v>100.23111479429932</v>
       </c>
       <c r="E73" t="n">
-        <v>42.198220154844364</v>
+        <v>47.300583582922719</v>
       </c>
       <c r="F73" t="n">
-        <v>10.338150332410137</v>
+        <v>11.691997073018198</v>
       </c>
       <c r="G73" t="n">
-        <v>19.020242843678158</v>
+        <v>21.196916081241778</v>
       </c>
     </row>
     <row r="74">
@@ -1837,19 +1837,19 @@
         <v>72</v>
       </c>
       <c r="C74" t="n">
-        <v>6.1762051960467108</v>
+        <v>6.8224519096385521</v>
       </c>
       <c r="D74" t="n">
-        <v>90.683639216796649</v>
+        <v>101.61701357542768</v>
       </c>
       <c r="E74" t="n">
-        <v>42.75645435536957</v>
+        <v>47.928020277148818</v>
       </c>
       <c r="F74" t="n">
-        <v>10.486615315566848</v>
+        <v>11.860336957347766</v>
       </c>
       <c r="G74" t="n">
-        <v>19.288350372485183</v>
+        <v>21.496206422495607</v>
       </c>
     </row>
     <row r="75">
@@ -1860,19 +1860,19 @@
         <v>73</v>
       </c>
       <c r="C75" t="n">
-        <v>6.2628703615324968</v>
+        <v>6.9179983267406948</v>
       </c>
       <c r="D75" t="n">
-        <v>91.932904990257853</v>
+        <v>103.02067195314409</v>
       </c>
       <c r="E75" t="n">
-        <v>43.321497691892105</v>
+        <v>48.563243890639441</v>
       </c>
       <c r="F75" t="n">
-        <v>10.637020994815945</v>
+        <v>12.030902009980602</v>
       </c>
       <c r="G75" t="n">
-        <v>19.559913668480441</v>
+        <v>21.799389061650785</v>
       </c>
     </row>
     <row r="76">
@@ -1883,19 +1883,19 @@
         <v>74</v>
       </c>
       <c r="C76" t="n">
-        <v>6.3506075882617603</v>
+        <v>7.0147500285872315</v>
       </c>
       <c r="D76" t="n">
-        <v>93.198008271391586</v>
+        <v>104.44227773949643</v>
       </c>
       <c r="E76" t="n">
-        <v>43.89341883490885</v>
+        <v>49.206317812935779</v>
       </c>
       <c r="F76" t="n">
-        <v>10.789390148947925</v>
+        <v>12.203715204248025</v>
       </c>
       <c r="G76" t="n">
-        <v>19.834971507303841</v>
+        <v>22.106503749707773</v>
       </c>
     </row>
     <row r="77">
@@ -1906,19 +1906,19 @@
         <v>75</v>
       </c>
       <c r="C77" t="n">
-        <v>6.4394288754632747</v>
+        <v>7.1127162368732941</v>
       </c>
       <c r="D77" t="n">
-        <v>94.479130585260847</v>
+        <v>105.88203385620264</v>
       </c>
       <c r="E77" t="n">
-        <v>44.472291489858847</v>
+        <v>49.857313129698106</v>
       </c>
       <c r="F77" t="n">
-        <v>10.943746040556844</v>
+        <v>12.378801598023365</v>
       </c>
       <c r="G77" t="n">
-        <v>20.113563929067684</v>
+        <v>22.41759457638997</v>
       </c>
     </row>
     <row r="78">
@@ -1929,19 +1929,19 @@
         <v>76</v>
       </c>
       <c r="C78" t="n">
-        <v>6.5293465124237429</v>
+        <v>7.2119074659004623</v>
       </c>
       <c r="D78" t="n">
-        <v>95.7764602681182</v>
+        <v>107.34013721092718</v>
       </c>
       <c r="E78" t="n">
-        <v>45.058190687916884</v>
+        <v>50.516308360899757</v>
       </c>
       <c r="F78" t="n">
-        <v>11.100112654330331</v>
+        <v>12.556185693898724</v>
       </c>
       <c r="G78" t="n">
-        <v>20.395732894189461</v>
+        <v>22.732703393178873</v>
       </c>
     </row>
     <row r="79">
@@ -1952,19 +1952,19 @@
         <v>77</v>
       </c>
       <c r="C79" t="n">
-        <v>6.6203730348768186</v>
+        <v>7.3123350786986174</v>
       </c>
       <c r="D79" t="n">
-        <v>97.090180012332908</v>
+        <v>108.90561842523684</v>
       </c>
       <c r="E79" t="n">
-        <v>45.651196487899718</v>
+        <v>51.183382524689037</v>
       </c>
       <c r="F79" t="n">
-        <v>11.258513274880087</v>
+        <v>12.772278628666463</v>
       </c>
       <c r="G79" t="n">
-        <v>20.681518399818209</v>
+        <v>23.066913840535868</v>
       </c>
     </row>
     <row r="80">
@@ -1975,19 +1975,19 @@
         <v>78</v>
       </c>
       <c r="C80" t="n">
-        <v>6.7125209077006618</v>
+        <v>7.4161777459379339</v>
       </c>
       <c r="D80" t="n">
-        <v>98.42047918347771</v>
+        <v>110.49873757208039</v>
       </c>
       <c r="E80" t="n">
-        <v>46.251388151153407</v>
+        <v>51.867414831462</v>
       </c>
       <c r="F80" t="n">
-        <v>11.41897184241428</v>
+        <v>12.99201205807006</v>
       </c>
       <c r="G80" t="n">
-        <v>20.970962346276188</v>
+        <v>23.407770564799499</v>
       </c>
     </row>
     <row r="81">
@@ -1998,19 +1998,19 @@
         <v>79</v>
       </c>
       <c r="C81" t="n">
-        <v>6.8058026444461532</v>
+        <v>7.5229113049834844</v>
       </c>
       <c r="D81" t="n">
-        <v>99.767547567512352</v>
+        <v>112.11705513439824</v>
       </c>
       <c r="E81" t="n">
-        <v>46.858846541515014</v>
+        <v>52.565812083505264</v>
       </c>
       <c r="F81" t="n">
-        <v>11.581512284783118</v>
+        <v>13.215347879647185</v>
       </c>
       <c r="G81" t="n">
-        <v>21.264106574865195</v>
+        <v>23.754518132833574</v>
       </c>
     </row>
     <row r="82">
@@ -2021,19 +2021,19 @@
         <v>80</v>
       </c>
       <c r="C82" t="n">
-        <v>6.9002307490798565</v>
+        <v>7.6321751624421283</v>
       </c>
       <c r="D82" t="n">
-        <v>101.13157618451446</v>
+        <v>113.7598909789249</v>
       </c>
       <c r="E82" t="n">
-        <v>47.473653955932633</v>
+        <v>53.277080281820368</v>
       </c>
       <c r="F82" t="n">
-        <v>11.746158673928008</v>
+        <v>13.442312732222559</v>
       </c>
       <c r="G82" t="n">
-        <v>21.56099321489933</v>
+        <v>24.106872106977626</v>
       </c>
     </row>
     <row r="83">
@@ -2044,19 +2044,19 @@
         <v>81</v>
       </c>
       <c r="C83" t="n">
-        <v>6.9958176474660689</v>
+        <v>7.7437229781791688</v>
       </c>
       <c r="D83" t="n">
-        <v>102.51275731340982</v>
+        <v>115.42701565979667</v>
       </c>
       <c r="E83" t="n">
-        <v>48.09589051172717</v>
+        <v>54.000229129637987</v>
       </c>
       <c r="F83" t="n">
-        <v>11.912935003294402</v>
+        <v>13.672960482380137</v>
       </c>
       <c r="G83" t="n">
-        <v>21.861664340544635</v>
+        <v>24.46469646779412</v>
       </c>
     </row>
     <row r="84">
@@ -2067,19 +2067,19 @@
         <v>82</v>
       </c>
       <c r="C84" t="n">
-        <v>7.0925759769885035</v>
+        <v>7.8573892370721836</v>
       </c>
       <c r="D84" t="n">
-        <v>103.91127985908633</v>
+        <v>164.59428205278257</v>
       </c>
       <c r="E84" t="n">
-        <v>48.725655746592459</v>
+        <v>8.2632342017512617</v>
       </c>
       <c r="F84" t="n">
-        <v>12.081866464046467</v>
+        <v>14.717581014321352</v>
       </c>
       <c r="G84" t="n">
-        <v>22.166162529054091</v>
+        <v>58.749064007990235</v>
       </c>
     </row>
     <row r="85">
@@ -2090,19 +2090,19 @@
         <v>83</v>
       </c>
       <c r="C85" t="n">
-        <v>7.1905166957180091</v>
+        <v>9.7423031110246008</v>
       </c>
       <c r="D85" t="n">
-        <v>105.32735031860479</v>
+        <v>132.13255820830275</v>
       </c>
       <c r="E85" t="n">
-        <v>49.362983284972458</v>
+        <v>61.792640214033732</v>
       </c>
       <c r="F85" t="n">
-        <v>12.252975251522017</v>
+        <v>15.885447524836875</v>
       </c>
       <c r="G85" t="n">
-        <v>22.47453056411717</v>
+        <v>28.049449273349776</v>
       </c>
     </row>
     <row r="86">
@@ -2113,19 +2113,19 @@
         <v>84</v>
       </c>
       <c r="C86" t="n">
-        <v>7.2896555337388556</v>
+        <v>9.7646775315765417</v>
       </c>
       <c r="D86" t="n">
-        <v>106.76117601604608</v>
+        <v>131.33695740858104</v>
       </c>
       <c r="E86" t="n">
-        <v>50.008014625163646</v>
+        <v>61.969993825039708</v>
       </c>
       <c r="F86" t="n">
-        <v>12.426289007657687</v>
+        <v>15.764046115948801</v>
       </c>
       <c r="G86" t="n">
-        <v>22.786816753162338</v>
+        <v>27.975421871561341</v>
       </c>
     </row>
     <row r="87">
@@ -2136,19 +2136,19 @@
         <v>85</v>
       </c>
       <c r="C87" t="n">
-        <v>7.3900034746580836</v>
+        <v>9.7405375200615332</v>
       </c>
       <c r="D87" t="n">
-        <v>108.21293753721785</v>
+        <v>134.50020821877527</v>
       </c>
       <c r="E87" t="n">
-        <v>50.660816045238803</v>
+        <v>63.378169644888317</v>
       </c>
       <c r="F87" t="n">
-        <v>12.601831469798771</v>
+        <v>16.130811022764565</v>
       </c>
       <c r="G87" t="n">
-        <v>23.103059838782247</v>
+        <v>28.617698709200532</v>
       </c>
     </row>
     <row r="88">
@@ -2159,19 +2159,19 @@
         <v>86</v>
       </c>
       <c r="C88" t="n">
-        <v>7.4915726661752302</v>
+        <v>9.7387957855083513</v>
       </c>
       <c r="D88" t="n">
-        <v>109.68284069151622</v>
+        <v>137.58100286457514</v>
       </c>
       <c r="E88" t="n">
-        <v>51.321462529276133</v>
+        <v>64.671257507088526</v>
       </c>
       <c r="F88" t="n">
-        <v>12.779627171126998</v>
+        <v>16.46480160706437</v>
       </c>
       <c r="G88" t="n">
-        <v>23.423304415958611</v>
+        <v>29.235096987252966</v>
       </c>
     </row>
     <row r="89">
@@ -2182,19 +2182,19 @@
         <v>87</v>
       </c>
       <c r="C89" t="n">
-        <v>7.5943763590774207</v>
+        <v>9.7649574589886043</v>
       </c>
       <c r="D89" t="n">
-        <v>111.17109440835596</v>
+        <v>140.43610403414846</v>
       </c>
       <c r="E89" t="n">
-        <v>51.990052890146615</v>
+        <v>65.918980058510897</v>
       </c>
       <c r="F89" t="n">
-        <v>12.959701939211993</v>
+        <v>16.79099892139952</v>
       </c>
       <c r="G89" t="n">
-        <v>23.747596733286741</v>
+        <v>29.830321214117074</v>
       </c>
     </row>
     <row r="90">
@@ -2205,19 +2205,19 @@
         <v>88</v>
       </c>
       <c r="C90" t="n">
-        <v>7.6984269700147907</v>
+        <v>9.8082825612796682</v>
       </c>
       <c r="D90" t="n">
-        <v>112.67789857307334</v>
+        <v>143.4064843827924</v>
       </c>
       <c r="E90" t="n">
-        <v>52.66666861351122</v>
+        <v>67.177309052585841</v>
       </c>
       <c r="F90" t="n">
-        <v>13.142081028594946</v>
+        <v>17.135251495206841</v>
       </c>
       <c r="G90" t="n">
-        <v>24.075980372606605</v>
+        <v>30.443915109202091</v>
       </c>
     </row>
     <row r="91">
@@ -2228,19 +2228,19 @@
         <v>89</v>
       </c>
       <c r="C91" t="n">
-        <v>7.8037373124460121</v>
+        <v>9.8736011501165812</v>
       </c>
       <c r="D91" t="n">
-        <v>114.20346171605318</v>
+        <v>146.38048081484254</v>
       </c>
       <c r="E91" t="n">
-        <v>53.3513987649496</v>
+        <v>68.248156003219677</v>
       </c>
       <c r="F91" t="n">
-        <v>13.326790055752483</v>
+        <v>17.487998513409924</v>
       </c>
       <c r="G91" t="n">
-        <v>24.408500889358564</v>
+        <v>31.052437118409802</v>
       </c>
     </row>
     <row r="92">
@@ -2251,19 +2251,19 @@
         <v>90</v>
       </c>
       <c r="C92" t="n">
-        <v>7.9103202540171393</v>
+        <v>9.9720545296784699</v>
       </c>
       <c r="D92" t="n">
-        <v>115.74799334321808</v>
+        <v>148.94294721379893</v>
       </c>
       <c r="E92" t="n">
-        <v>54.04433224710526</v>
+        <v>69.14027401974873</v>
       </c>
       <c r="F92" t="n">
-        <v>13.513854943169639</v>
+        <v>17.808646571442267</v>
       </c>
       <c r="G92" t="n">
-        <v>24.745204099135709</v>
+        <v>31.613003829315915</v>
       </c>
     </row>
     <row r="93">
@@ -2274,19 +2274,19 @@
         <v>91</v>
       </c>
       <c r="C93" t="n">
-        <v>8.0181887438290733</v>
+        <v>10.093848884010907</v>
       </c>
       <c r="D93" t="n">
-        <v>117.31170392401211</v>
+        <v>151.17270175665956</v>
       </c>
       <c r="E93" t="n">
-        <v>54.745559062962336</v>
+        <v>70.036132329908909</v>
       </c>
       <c r="F93" t="n">
-        <v>13.703301734060563</v>
+        <v>18.109167972025293</v>
       </c>
       <c r="G93" t="n">
-        <v>25.086135917725258</v>
+        <v>32.08610998659762</v>
       </c>
     </row>
     <row r="94">
@@ -2297,19 +2297,19 @@
         <v>92</v>
       </c>
       <c r="C94" t="n">
-        <v>8.1273557925346331</v>
+        <v>10.226754037951331</v>
       </c>
       <c r="D94" t="n">
-        <v>118.89480785805384</v>
+        <v>153.37574156596492</v>
       </c>
       <c r="E94" t="n">
-        <v>55.455169387664121</v>
+        <v>70.953887914380942</v>
       </c>
       <c r="F94" t="n">
-        <v>13.895156897481955</v>
+        <v>18.411569223855082</v>
       </c>
       <c r="G94" t="n">
-        <v>25.431343254652539</v>
+        <v>32.552764647069687</v>
       </c>
     </row>
     <row r="95">
@@ -2320,19 +2320,19 @@
         <v>93</v>
       </c>
       <c r="C95" t="n">
-        <v>8.2378345276366414</v>
+        <v>10.366425508303026</v>
       </c>
       <c r="D95" t="n">
-        <v>120.49751844081246</v>
+        <v>155.62697310260484</v>
       </c>
       <c r="E95" t="n">
-        <v>56.173255348868977</v>
+        <v>71.906008988690814</v>
       </c>
       <c r="F95" t="n">
-        <v>14.089446800674072</v>
+        <v>18.721244370390934</v>
       </c>
       <c r="G95" t="n">
-        <v>25.780872474922418</v>
+        <v>33.032280951315769</v>
       </c>
     </row>
     <row r="96">
@@ -2343,19 +2343,19 @@
         <v>94</v>
       </c>
       <c r="C96" t="n">
-        <v>8.3496381117487104</v>
+        <v>10.510872941748259</v>
       </c>
       <c r="D96" t="n">
-        <v>122.12005427239239</v>
+        <v>157.91946634658072</v>
       </c>
       <c r="E96" t="n">
-        <v>56.899908750879206</v>
+        <v>72.883782056688034</v>
       </c>
       <c r="F96" t="n">
-        <v>14.286198374603032</v>
+        <v>19.037491411711716</v>
       </c>
       <c r="G96" t="n">
-        <v>26.134771362324901</v>
+        <v>33.521845459126006</v>
       </c>
     </row>
     <row r="97">
@@ -2366,19 +2366,19 @@
         <v>95</v>
       </c>
       <c r="C97" t="n">
-        <v>8.4627798371595766</v>
+        <v>10.659028220977396</v>
       </c>
       <c r="D97" t="n">
-        <v>123.76263152320089</v>
+        <v>160.2493260238102</v>
       </c>
       <c r="E97" t="n">
-        <v>57.63522751630012</v>
+        <v>73.882231455793729</v>
       </c>
       <c r="F97" t="n">
-        <v>14.485438676975292</v>
+        <v>19.359882541564346</v>
       </c>
       <c r="G97" t="n">
-        <v>26.493087289398282</v>
+        <v>34.020005638756992</v>
       </c>
     </row>
     <row r="98">
@@ -2389,19 +2389,19 @@
         <v>96</v>
       </c>
       <c r="C98" t="n">
-        <v>8.5772725982455267</v>
+        <v>10.810286137374344</v>
       </c>
       <c r="D98" t="n">
-        <v>125.42547228831326</v>
+        <v>162.61437459823171</v>
       </c>
       <c r="E98" t="n">
-        <v>58.379290661866825</v>
+        <v>74.898402040146394</v>
       </c>
       <c r="F98" t="n">
-        <v>14.687194121291013</v>
+        <v>19.688162959268968</v>
       </c>
       <c r="G98" t="n">
-        <v>26.85586721727433</v>
+        <v>34.525979888617158</v>
       </c>
     </row>
     <row r="99">
@@ -2412,19 +2412,19 @@
         <v>97</v>
       </c>
       <c r="C99" t="n">
-        <v>8.6931308398549465</v>
+        <v>10.964299078231186</v>
       </c>
       <c r="D99" t="n">
-        <v>127.10880658869438</v>
+        <v>165.01343932177116</v>
       </c>
       <c r="E99" t="n">
-        <v>59.132211786125481</v>
+        <v>75.930529248392517</v>
       </c>
       <c r="F99" t="n">
-        <v>14.891493365894863</v>
+        <v>20.022191517337031</v>
       </c>
       <c r="G99" t="n">
-        <v>27.223162819701805</v>
+        <v>35.039350667939352</v>
       </c>
     </row>
     <row r="100">
@@ -2435,19 +2435,19 @@
         <v>98</v>
       </c>
       <c r="C100" t="n">
-        <v>8.8103675327145226</v>
+        <v>11.120868273658322</v>
       </c>
       <c r="D100" t="n">
-        <v>128.81285013288124</v>
+        <v>167.44593508710307</v>
       </c>
       <c r="E100" t="n">
-        <v>59.894078749619958</v>
+        <v>76.977573472451255</v>
       </c>
       <c r="F100" t="n">
-        <v>15.098363365704522</v>
+        <v>20.361901489692798</v>
       </c>
       <c r="G100" t="n">
-        <v>27.595020183998614</v>
+        <v>35.559902033941917</v>
       </c>
     </row>
     <row r="101">
@@ -2458,19 +2458,19 @@
         <v>99</v>
       </c>
       <c r="C101" t="n">
-        <v>8.9289962692441733</v>
+        <v>11.279882380715346</v>
       </c>
       <c r="D101" t="n">
-        <v>130.53783262758068</v>
+        <v>169.9116331370343</v>
       </c>
       <c r="E101" t="n">
-        <v>60.664989041216174</v>
+        <v>78.038938560627884</v>
       </c>
       <c r="F101" t="n">
-        <v>15.307832050414998</v>
+        <v>20.707276301394273</v>
       </c>
       <c r="G101" t="n">
-        <v>27.9714892080402</v>
+        <v>36.087534628805265</v>
       </c>
     </row>
   </sheetData>

</xml_diff>